<commit_message>
documentação sobre as funcionalidades implementadas.
</commit_message>
<xml_diff>
--- a/Documentação/auto-avaliacao_do_grupo.xlsx
+++ b/Documentação/auto-avaliacao_do_grupo.xlsx
@@ -607,14 +607,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
@@ -936,8 +941,9 @@
     <mergeCell ref="C8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>